<commit_message>
power of kth element
</commit_message>
<xml_diff>
--- a/Data Structure/recursion/Recursion.xlsx
+++ b/Data Structure/recursion/Recursion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shubhamrathod/Documents/Study Material/DS/DataStructure-And-Algorithm/Data Structure/recursion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E16D6C-EF54-6E4E-B404-8BF4BCD096A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99836903-B631-6548-9CA6-BB2FDE0A3B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4E42177B-4881-CA45-8674-08098C02AC7A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Number</t>
   </si>
@@ -225,6 +225,78 @@
     <t>Power Of Two</t>
   </si>
   <si>
+    <t>Power of Three</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Approach 1 ---&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Common For all:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Power Of K:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    class Solution:
+    def isPowerOfTwo(self, n: int) -&gt; bool:
+        if n == 0:
+            return False
+        while n % k == 0:
+            n /= k
+        return n == 1</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -320,7 +392,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Bit Wise:</t>
+      <t>Approach Two. -- &gt; Bit Wise:</t>
     </r>
     <r>
       <rPr>
@@ -334,6 +406,38 @@
     def isPowerOfTwo(self, n: int) -&gt; bool:
         if n == 0: return False
         return n &amp; (n-1) == 0</t>
+    </r>
+  </si>
+  <si>
+    <t>Power OF Four</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Approach 1 ---&gt; Common For all:
+Power Of K:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    class Solution:
+    def isPowerOfTwo(self, n: int) -&gt; bool:
+        if n == 0:
+            return False
+        while n % k == 0:
+            n /= k
+        return n == 1</t>
     </r>
   </si>
 </sst>
@@ -770,8 +874,8 @@
   <dimension ref="A1:C284"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <pane ySplit="5" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -857,18 +961,30 @@
         <v>11</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="235" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="C10" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="189" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>

</xml_diff>